<commit_message>
Modificaciones en Plan de trabajo
Incluidos puntos que se han ido comentando en el plan de trabajo, y modificadas fechas revisión dataset. Todos los cambios con letra en lila, para revisar y comentar en sesión de equipo.
</commit_message>
<xml_diff>
--- a/doc/Copia de Formato plan de trabajo AI Saturdays (2).xlsx
+++ b/doc/Copia de Formato plan de trabajo AI Saturdays (2).xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="55">
   <si>
     <t>Actividad</t>
   </si>
@@ -192,6 +192,18 @@
   <si>
     <t>5 semanas</t>
   </si>
+  <si>
+    <t>4 semanas</t>
+  </si>
+  <si>
+    <t>Mejorar chatbot. Incluir botones opciones, dislpay de las respuestas</t>
+  </si>
+  <si>
+    <t>Punto de situación - Mentoría</t>
+  </si>
+  <si>
+    <t>TBD</t>
+  </si>
 </sst>
 </file>
 
@@ -200,7 +212,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/m/yyyy"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -286,6 +298,12 @@
       <sz val="14"/>
       <color rgb="FF1155CC"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF7030A0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -431,7 +449,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -544,11 +562,42 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="17">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF6D9EEB"/>
+          <bgColor rgb="FF6D9EEB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF6D9EEB"/>
+          <bgColor rgb="FF6D9EEB"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF999999"/>
@@ -563,8 +612,8 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FF1155CC"/>
-          <bgColor rgb="FF1155CC"/>
+          <fgColor rgb="FF6D9EEB"/>
+          <bgColor rgb="FF6D9EEB"/>
         </patternFill>
       </fill>
     </dxf>
@@ -573,6 +622,102 @@
         <patternFill patternType="solid">
           <fgColor rgb="FF6D9EEB"/>
           <bgColor rgb="FF6D9EEB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF6D9EEB"/>
+          <bgColor rgb="FF6D9EEB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF6D9EEB"/>
+          <bgColor rgb="FF6D9EEB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF6D9EEB"/>
+          <bgColor rgb="FF6D9EEB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF6D9EEB"/>
+          <bgColor rgb="FF6D9EEB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF6D9EEB"/>
+          <bgColor rgb="FF6D9EEB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF6D9EEB"/>
+          <bgColor rgb="FF6D9EEB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF6D9EEB"/>
+          <bgColor rgb="FF6D9EEB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF6D9EEB"/>
+          <bgColor rgb="FF6D9EEB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF6D9EEB"/>
+          <bgColor rgb="FF6D9EEB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF6D9EEB"/>
+          <bgColor rgb="FF6D9EEB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF6D9EEB"/>
+          <bgColor rgb="FF6D9EEB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF1155CC"/>
+          <bgColor rgb="FF1155CC"/>
         </patternFill>
       </fill>
     </dxf>
@@ -789,7 +934,7 @@
   </sheetPr>
   <dimension ref="A1:Y1002"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -797,8 +942,15 @@
     <col min="2" max="2" width="13.25" customWidth="1"/>
     <col min="3" max="4" width="13.25" hidden="1" customWidth="1"/>
     <col min="5" max="5" width="10.875" customWidth="1"/>
-    <col min="6" max="6" width="10" customWidth="1"/>
-    <col min="7" max="20" width="9.5" customWidth="1"/>
+    <col min="6" max="6" width="10.75" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.5" customWidth="1"/>
+    <col min="8" max="9" width="10.125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.25" bestFit="1" customWidth="1"/>
+    <col min="11" max="13" width="10.125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.25" bestFit="1" customWidth="1"/>
+    <col min="15" max="18" width="10.125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="8.25" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.25" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="9.5" hidden="1" customWidth="1"/>
     <col min="22" max="25" width="9.5" customWidth="1"/>
   </cols>
@@ -1535,16 +1687,16 @@
       <c r="A13" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="B13" s="23" t="s">
-        <v>46</v>
+      <c r="B13" s="42" t="s">
+        <v>50</v>
       </c>
       <c r="C13" s="23"/>
       <c r="D13" s="23"/>
-      <c r="E13" s="24">
+      <c r="E13" s="41">
         <v>44885</v>
       </c>
-      <c r="F13" s="24">
-        <v>44899</v>
+      <c r="F13" s="41">
+        <v>44911</v>
       </c>
       <c r="G13" s="10"/>
       <c r="H13" s="25" t="s">
@@ -1569,10 +1721,10 @@
         <v>42</v>
       </c>
       <c r="O13" s="26" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="P13" s="26" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="Q13" s="26" t="s">
         <v>43</v>
@@ -1897,17 +2049,21 @@
       <c r="X18" s="10"/>
       <c r="Y18" s="10"/>
     </row>
-    <row r="19" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="31" t="s">
-        <v>28</v>
-      </c>
-      <c r="B19" s="23" t="s">
-        <v>48</v>
-      </c>
-      <c r="C19" s="23"/>
-      <c r="D19" s="23"/>
-      <c r="E19" s="29"/>
-      <c r="F19" s="29"/>
+    <row r="19" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A19" s="38" t="s">
+        <v>52</v>
+      </c>
+      <c r="B19" s="39" t="s">
+        <v>51</v>
+      </c>
+      <c r="C19" s="39"/>
+      <c r="D19" s="39"/>
+      <c r="E19" s="40">
+        <v>44907</v>
+      </c>
+      <c r="F19" s="40">
+        <v>44925</v>
+      </c>
       <c r="G19" s="10"/>
       <c r="H19" s="25" t="s">
         <v>43</v>
@@ -1931,13 +2087,13 @@
         <v>43</v>
       </c>
       <c r="O19" s="26" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="P19" s="26" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="Q19" s="26" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="R19" s="26" t="s">
         <v>43</v>
@@ -1954,17 +2110,21 @@
       <c r="X19" s="10"/>
       <c r="Y19" s="10"/>
     </row>
-    <row r="20" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="31" t="s">
-        <v>28</v>
-      </c>
-      <c r="B20" s="23" t="s">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A20" s="38" t="s">
+        <v>53</v>
+      </c>
+      <c r="B20" s="39" t="s">
         <v>48</v>
       </c>
-      <c r="C20" s="23"/>
-      <c r="D20" s="23"/>
-      <c r="E20" s="29"/>
-      <c r="F20" s="29"/>
+      <c r="C20" s="39"/>
+      <c r="D20" s="39"/>
+      <c r="E20" s="40" t="s">
+        <v>54</v>
+      </c>
+      <c r="F20" s="40" t="s">
+        <v>54</v>
+      </c>
       <c r="G20" s="10"/>
       <c r="H20" s="25" t="s">
         <v>43</v>
@@ -1991,7 +2151,7 @@
         <v>43</v>
       </c>
       <c r="P20" s="26" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="Q20" s="26" t="s">
         <v>43</v>
@@ -28872,25 +29032,50 @@
       <c r="Y1002" s="10"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="H4:T8 H12:T18 H28:T31">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+  <conditionalFormatting sqref="H4:T8 H28:T31 H12:T18">
+    <cfRule type="cellIs" dxfId="3" priority="7" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3:T3 H11:T11 H27:T27">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="8" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:U2">
-    <cfRule type="expression" dxfId="0" priority="3">
+    <cfRule type="expression" dxfId="2" priority="9">
       <formula>AND(ISNUMBER(H2),TRUNC(H2)&lt;TODAY())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O19">
+    <cfRule type="cellIs" dxfId="15" priority="6" operator="equal">
+      <formula>"x"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P19">
+    <cfRule type="cellIs" dxfId="13" priority="5" operator="equal">
+      <formula>"x"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q19">
+    <cfRule type="cellIs" dxfId="11" priority="4" operator="equal">
+      <formula>"x"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R19">
+    <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
+      <formula>"x"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P20">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+      <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup fitToHeight="0" orientation="landscape"/>
+  <pageSetup fitToHeight="0" orientation="landscape" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>